<commit_message>
Add solution for example 3 margin
</commit_message>
<xml_diff>
--- a/Tabellen/Beispiel1_N.xlsx
+++ b/Tabellen/Beispiel1_N.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEV\Git\SchulzeMethode\Tabellen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67F3685E-3F4A-4332-8301-510F4BDF100C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A91940-419B-4E36-9578-76D39C821575}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" xr2:uid="{F2AABF5E-7F7E-4D50-9658-5E2C6FE54334}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="22">
   <si>
     <t>---</t>
   </si>
@@ -57,6 +57,45 @@
   </si>
   <si>
     <t>N[d, *]</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>P[*,a]</t>
+  </si>
+  <si>
+    <t>P[*,b]</t>
+  </si>
+  <si>
+    <t>P[*,c]</t>
+  </si>
+  <si>
+    <t>P[*,d]</t>
+  </si>
+  <si>
+    <t>P[a, *]</t>
+  </si>
+  <si>
+    <t>P[b, *]</t>
+  </si>
+  <si>
+    <t>P[c, *]</t>
+  </si>
+  <si>
+    <t>P[d, *]</t>
   </si>
 </sst>
 </file>
@@ -322,7 +361,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -361,6 +400,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -675,16 +716,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{395652B2-B2ED-4DAC-8868-D3E28F537D3A}">
-  <dimension ref="B3:F8"/>
+  <dimension ref="B3:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:F8"/>
+      <selection activeCell="H11" sqref="H11:L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="11"/>
       <c r="C4" s="12" t="s">
         <v>1</v>
@@ -698,8 +739,23 @@
       <c r="F4" s="14" t="s">
         <v>4</v>
       </c>
+      <c r="H4" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="L4" s="14" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B5" s="15" t="s">
         <v>5</v>
       </c>
@@ -715,8 +771,23 @@
       <c r="F5" s="3">
         <v>13</v>
       </c>
+      <c r="H5" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2">
+        <v>67</v>
+      </c>
+      <c r="K5" s="2">
+        <v>28</v>
+      </c>
+      <c r="L5" s="3">
+        <v>40</v>
+      </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" s="16" t="s">
         <v>6</v>
       </c>
@@ -732,8 +803,23 @@
       <c r="F6" s="7">
         <v>23</v>
       </c>
+      <c r="H6" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="4">
+        <v>55</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K6" s="6">
+        <v>79</v>
+      </c>
+      <c r="L6" s="7">
+        <v>58</v>
+      </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" s="16" t="s">
         <v>7</v>
       </c>
@@ -749,8 +835,23 @@
       <c r="F7" s="7">
         <v>4</v>
       </c>
+      <c r="H7" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="4">
+        <v>36</v>
+      </c>
+      <c r="J7" s="6">
+        <v>59</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="L7" s="7">
+        <v>45</v>
+      </c>
     </row>
-    <row r="8" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="17" t="s">
         <v>8</v>
       </c>
@@ -764,6 +865,180 @@
         <v>24</v>
       </c>
       <c r="F8" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="8">
+        <v>50</v>
+      </c>
+      <c r="J8" s="9">
+        <v>72</v>
+      </c>
+      <c r="K8" s="9">
+        <v>29</v>
+      </c>
+      <c r="L8" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>12</v>
+      </c>
+      <c r="E11">
+        <v>12</v>
+      </c>
+      <c r="F11">
+        <v>12</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="K11" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="L11" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B12" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>20</v>
+      </c>
+      <c r="F12">
+        <v>16</v>
+      </c>
+      <c r="H12" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J12" s="2">
+        <v>12</v>
+      </c>
+      <c r="K12" s="2">
+        <v>12</v>
+      </c>
+      <c r="L12" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B13" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="D13">
+        <v>14</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>16</v>
+      </c>
+      <c r="H13" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" s="4">
+        <v>10</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K13" s="6">
+        <v>20</v>
+      </c>
+      <c r="L13" s="7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B14" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <v>14</v>
+      </c>
+      <c r="E14">
+        <v>14</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H14" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I14" s="4">
+        <v>10</v>
+      </c>
+      <c r="J14" s="6">
+        <v>14</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="L14" s="7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H15" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I15" s="8">
+        <v>10</v>
+      </c>
+      <c r="J15" s="9">
+        <v>14</v>
+      </c>
+      <c r="K15" s="9">
+        <v>14</v>
+      </c>
+      <c r="L15" s="10" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>